<commit_message>
Update OpenHornet IO Requirements.xlsx
</commit_message>
<xml_diff>
--- a/ECAD/docs/OpenHornet IO Requirements.xlsx
+++ b/ECAD/docs/OpenHornet IO Requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\OpenHornet\ECAD\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D6E109D-B3DB-4F0A-B16D-A51BD2622E6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612A6C94-703F-44CB-89AC-3C09DB044313}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{140A0762-4383-4061-93A6-DED8B461E90E}"/>
+    <workbookView xWindow="2745" yWindow="2040" windowWidth="21600" windowHeight="12735" activeTab="1" xr2:uid="{140A0762-4383-4061-93A6-DED8B461E90E}"/>
   </bookViews>
   <sheets>
     <sheet name="IO Requirements" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="129">
   <si>
     <t>Master Arm</t>
   </si>
@@ -385,24 +385,12 @@
     <t>Mega-based USB</t>
   </si>
   <si>
-    <t>Cable</t>
-  </si>
-  <si>
-    <t>IFEI PCB -&gt; ABSIS Nano #3</t>
-  </si>
-  <si>
     <t>Cable -&gt; RS485 Slave</t>
   </si>
   <si>
     <t>Cable -&gt; UFC</t>
   </si>
   <si>
-    <t>ABSIS Nano #3</t>
-  </si>
-  <si>
-    <t>AMPCD Button Board -&gt; Nano #4</t>
-  </si>
-  <si>
     <t>Master Arm Backlight PCB -&gt; ABSIS Nano #1</t>
   </si>
   <si>
@@ -410,6 +398,30 @@
   </si>
   <si>
     <t>Spin PCB -&gt; ABSIS Nano #4</t>
+  </si>
+  <si>
+    <t>IFEI PCB -&gt; ABSIS Nano #5</t>
+  </si>
+  <si>
+    <t>ABSIS Nano #5</t>
+  </si>
+  <si>
+    <t>RWR Control PCB</t>
+  </si>
+  <si>
+    <t>Backlighting PCB won't have room for in-out standard connectors, so this may need to be on a dedicated channel. Requires 4x PWM pins to control VID29.</t>
+  </si>
+  <si>
+    <t>AMPCD Button Board -&gt; ABSIS Nano #6</t>
+  </si>
+  <si>
+    <t>ECM Jett PCB -&gt; ABSIS Nano #7</t>
+  </si>
+  <si>
+    <t>Wire to ABSIS Nano #7</t>
+  </si>
+  <si>
+    <t>ABSIS Nano #8</t>
   </si>
 </sst>
 </file>
@@ -477,10 +489,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2193,8 +2201,8 @@
   <dimension ref="A1:T66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T11" sqref="T11"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2298,10 +2306,10 @@
         <v>45</v>
       </c>
       <c r="R2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="S2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="T2" t="s">
         <v>29</v>
@@ -2400,7 +2408,7 @@
         <v>107</v>
       </c>
       <c r="S5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="T5" t="s">
         <v>29</v>
@@ -2470,7 +2478,7 @@
         <v>111</v>
       </c>
       <c r="S7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="T7" t="s">
         <v>19</v>
@@ -2502,7 +2510,7 @@
         <v>107</v>
       </c>
       <c r="S8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="T8" t="s">
         <v>29</v>
@@ -2563,7 +2571,7 @@
         <v>29</v>
       </c>
       <c r="R10" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="S10" t="s">
         <v>104</v>
@@ -2601,10 +2609,10 @@
         <v>34</v>
       </c>
       <c r="R11" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="S11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="T11" t="s">
         <v>29</v>
@@ -2694,7 +2702,7 @@
         <v>39</v>
       </c>
       <c r="R15" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="S15" t="s">
         <v>116</v>
@@ -2726,16 +2734,16 @@
         <v>19</v>
       </c>
       <c r="R16" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="S16" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="T16" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -2758,10 +2766,16 @@
         <v>29</v>
       </c>
       <c r="R17" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="S17" t="s">
+        <v>116</v>
+      </c>
+      <c r="T17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -2786,8 +2800,17 @@
       <c r="P18" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R18" t="s">
+        <v>123</v>
+      </c>
+      <c r="S18" t="s">
+        <v>103</v>
+      </c>
+      <c r="T18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>44</v>
       </c>
@@ -2807,13 +2830,22 @@
         <v>29</v>
       </c>
       <c r="P19" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="Q19" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R19" t="s">
+        <v>126</v>
+      </c>
+      <c r="S19" t="s">
+        <v>116</v>
+      </c>
+      <c r="T19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>46</v>
       </c>
@@ -2833,10 +2865,19 @@
         <v>19</v>
       </c>
       <c r="Q20" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="R20" t="s">
+        <v>127</v>
+      </c>
+      <c r="S20" t="s">
+        <v>116</v>
+      </c>
+      <c r="T20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -2864,8 +2905,17 @@
       <c r="Q21" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R21" t="s">
+        <v>128</v>
+      </c>
+      <c r="S21" t="s">
+        <v>116</v>
+      </c>
+      <c r="T21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -2894,7 +2944,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>53</v>
       </c>
@@ -2917,7 +2967,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>54</v>
       </c>
@@ -2937,7 +2987,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>55</v>
       </c>
@@ -2957,7 +3007,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>57</v>
       </c>
@@ -2977,7 +3027,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>58</v>
       </c>
@@ -2997,7 +3047,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>59</v>
       </c>
@@ -3017,7 +3067,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>60</v>
       </c>
@@ -3040,7 +3090,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>61</v>
       </c>
@@ -3066,7 +3116,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
DDI WIP, various updates
DDI WIP
Documentation updates
Added missing right console PCB/MCAD
</commit_message>
<xml_diff>
--- a/ECAD/docs/OpenHornet IO Requirements.xlsx
+++ b/ECAD/docs/OpenHornet IO Requirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\OpenHornet\ECAD\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\OpenHornet\ECAD\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612A6C94-703F-44CB-89AC-3C09DB044313}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC4D9E3-E070-4BE4-B5DA-2E31DF2D9594}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2745" yWindow="2040" windowWidth="21600" windowHeight="12735" activeTab="1" xr2:uid="{140A0762-4383-4061-93A6-DED8B461E90E}"/>
+    <workbookView xWindow="-27630" yWindow="1170" windowWidth="21600" windowHeight="12735" activeTab="1" xr2:uid="{140A0762-4383-4061-93A6-DED8B461E90E}"/>
   </bookViews>
   <sheets>
     <sheet name="IO Requirements" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="129">
   <si>
     <t>Master Arm</t>
   </si>
@@ -453,7 +453,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -461,11 +461,128 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -474,6 +591,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2198,11 +2329,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EE83AAF-46AE-4551-A6AC-8AAD93187AC6}">
-  <dimension ref="A1:T66"/>
+  <dimension ref="A1:T68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q23" sqref="Q23"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2916,28 +3047,36 @@
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="5">
         <v>4</v>
       </c>
-      <c r="G23">
-        <v>1</v>
-      </c>
-      <c r="H23">
-        <v>1</v>
-      </c>
-      <c r="N23" t="s">
-        <v>29</v>
-      </c>
-      <c r="O23" t="s">
-        <v>29</v>
-      </c>
-      <c r="P23" t="s">
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="13">
+        <v>1</v>
+      </c>
+      <c r="H23" s="13">
+        <v>1</v>
+      </c>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O23" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P23" s="6" t="s">
         <v>19</v>
       </c>
       <c r="Q23" t="s">
@@ -2945,838 +3084,1209 @@
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="8">
         <v>10</v>
       </c>
-      <c r="H24">
-        <v>2</v>
-      </c>
-      <c r="N24" t="s">
-        <v>29</v>
-      </c>
-      <c r="O24" t="s">
-        <v>29</v>
-      </c>
-      <c r="P24" t="s">
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14">
+        <v>2</v>
+      </c>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O24" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P24" s="9" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="J25">
-        <v>1</v>
-      </c>
-      <c r="N25" t="s">
-        <v>29</v>
-      </c>
-      <c r="O25" t="s">
-        <v>29</v>
-      </c>
-      <c r="P25" t="s">
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8">
+        <v>1</v>
+      </c>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O25" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P25" s="9" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="11">
         <v>3</v>
       </c>
-      <c r="N26" t="s">
-        <v>29</v>
-      </c>
-      <c r="O26" t="s">
-        <v>29</v>
-      </c>
-      <c r="P26" t="s">
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+      <c r="N26" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="O26" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="P26" s="12" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="8">
+        <v>2</v>
+      </c>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O27" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P27" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="N27" t="s">
-        <v>29</v>
-      </c>
-      <c r="O27" t="s">
-        <v>29</v>
-      </c>
-      <c r="P27" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q27" t="s">
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="8"/>
+      <c r="N28" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O28" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P28" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q28" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>58</v>
-      </c>
-      <c r="B28" t="s">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C28">
-        <v>2</v>
-      </c>
-      <c r="N28" t="s">
-        <v>29</v>
-      </c>
-      <c r="O28" t="s">
-        <v>29</v>
-      </c>
-      <c r="P28" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>59</v>
-      </c>
-      <c r="B29" t="s">
+      <c r="C29" s="8">
+        <v>1</v>
+      </c>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O29" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P29" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
-      <c r="N29" t="s">
-        <v>29</v>
-      </c>
-      <c r="O29" t="s">
-        <v>29</v>
-      </c>
-      <c r="P29" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>60</v>
-      </c>
-      <c r="B30" t="s">
+      <c r="C30" s="8">
+        <v>3</v>
+      </c>
+      <c r="D30" s="8">
+        <v>2</v>
+      </c>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="8"/>
+      <c r="N30" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O30" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P30" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C30">
+      <c r="C31" s="8">
         <v>3</v>
       </c>
-      <c r="D30">
-        <v>2</v>
-      </c>
-      <c r="N30" t="s">
-        <v>29</v>
-      </c>
-      <c r="O30" t="s">
-        <v>29</v>
-      </c>
-      <c r="P30" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>61</v>
-      </c>
-      <c r="B31" t="s">
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8">
+        <v>1</v>
+      </c>
+      <c r="H31" s="8">
+        <v>3</v>
+      </c>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="8"/>
+      <c r="M31" s="8"/>
+      <c r="N31" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O31" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P31" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C31">
+      <c r="C32" s="8">
+        <v>7</v>
+      </c>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8">
+        <v>1</v>
+      </c>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="8"/>
+      <c r="N32" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O32" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P32" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="8">
         <v>3</v>
       </c>
-      <c r="G31">
-        <v>1</v>
-      </c>
-      <c r="H31">
-        <v>1</v>
-      </c>
-      <c r="N31" t="s">
-        <v>29</v>
-      </c>
-      <c r="O31" t="s">
-        <v>29</v>
-      </c>
-      <c r="P31" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>63</v>
-      </c>
-      <c r="B32" t="s">
+      <c r="D33" s="8"/>
+      <c r="E33" s="8">
+        <v>1</v>
+      </c>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8">
+        <v>1</v>
+      </c>
+      <c r="L33" s="8"/>
+      <c r="M33" s="8"/>
+      <c r="N33" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O33" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P33" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C32">
-        <v>7</v>
-      </c>
-      <c r="H32">
-        <v>1</v>
-      </c>
-      <c r="N32" t="s">
-        <v>29</v>
-      </c>
-      <c r="O32" t="s">
-        <v>29</v>
-      </c>
-      <c r="P32" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>62</v>
-      </c>
-      <c r="B33" t="s">
+      <c r="C34" s="8">
+        <v>2</v>
+      </c>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="8"/>
+      <c r="N34" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O34" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P34" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C33">
+      <c r="C35" s="8">
+        <v>29</v>
+      </c>
+      <c r="D35" s="8">
+        <v>8</v>
+      </c>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="8"/>
+      <c r="L35" s="8"/>
+      <c r="M35" s="8"/>
+      <c r="N35" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O35" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P35" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" s="8">
         <v>3</v>
       </c>
-      <c r="E33">
-        <v>1</v>
-      </c>
-      <c r="K33">
-        <v>1</v>
-      </c>
-      <c r="N33" t="s">
-        <v>29</v>
-      </c>
-      <c r="O33" t="s">
-        <v>29</v>
-      </c>
-      <c r="P33" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>65</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="8"/>
+      <c r="M36" s="8"/>
+      <c r="N36" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O36" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P36" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C34">
-        <v>2</v>
-      </c>
-      <c r="N34" t="s">
-        <v>29</v>
-      </c>
-      <c r="O34" t="s">
-        <v>29</v>
-      </c>
-      <c r="P34" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>66</v>
-      </c>
-      <c r="B35" t="s">
+      <c r="C37" s="8">
+        <v>2</v>
+      </c>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
+      <c r="M37" s="8"/>
+      <c r="N37" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O37" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P37" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B38" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C35">
-        <v>29</v>
-      </c>
-      <c r="D35">
-        <v>8</v>
-      </c>
-      <c r="N35" t="s">
-        <v>29</v>
-      </c>
-      <c r="O35" t="s">
-        <v>29</v>
-      </c>
-      <c r="P35" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>67</v>
-      </c>
-      <c r="B36" t="s">
+      <c r="C38" s="8">
+        <v>1</v>
+      </c>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="8"/>
+      <c r="L38" s="8"/>
+      <c r="M38" s="8"/>
+      <c r="N38" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O38" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P38" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B39" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C36">
-        <v>3</v>
-      </c>
-      <c r="N36" t="s">
-        <v>29</v>
-      </c>
-      <c r="O36" t="s">
-        <v>29</v>
-      </c>
-      <c r="P36" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>68</v>
-      </c>
-      <c r="B37" t="s">
-        <v>12</v>
-      </c>
-      <c r="C37">
-        <v>2</v>
-      </c>
-      <c r="N37" t="s">
-        <v>29</v>
-      </c>
-      <c r="O37" t="s">
-        <v>29</v>
-      </c>
-      <c r="P37" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>69</v>
-      </c>
-      <c r="B38" t="s">
-        <v>12</v>
-      </c>
-      <c r="C38">
-        <v>1</v>
-      </c>
-      <c r="N38" t="s">
-        <v>29</v>
-      </c>
-      <c r="O38" t="s">
-        <v>29</v>
-      </c>
-      <c r="P38" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>70</v>
-      </c>
-      <c r="B39" t="s">
-        <v>12</v>
-      </c>
-      <c r="C39">
+      <c r="C39" s="8">
         <v>4</v>
       </c>
-      <c r="N39" t="s">
-        <v>29</v>
-      </c>
-      <c r="O39" t="s">
-        <v>29</v>
-      </c>
-      <c r="P39" t="s">
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="8"/>
+      <c r="M39" s="8"/>
+      <c r="N39" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O39" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P39" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="A40" s="8" t="s">
         <v>98</v>
+      </c>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="8"/>
+      <c r="K40" s="8"/>
+      <c r="L40" s="8"/>
+      <c r="M40" s="8"/>
+      <c r="N40" s="8"/>
+      <c r="O40" s="8"/>
+      <c r="P40" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="Q40" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="A41" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C41">
-        <v>1</v>
-      </c>
-      <c r="N41" t="s">
-        <v>29</v>
-      </c>
-      <c r="O41" t="s">
-        <v>29</v>
-      </c>
-      <c r="P41" t="s">
+      <c r="C41" s="8">
+        <v>1</v>
+      </c>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
+      <c r="K41" s="8"/>
+      <c r="L41" s="8"/>
+      <c r="M41" s="8"/>
+      <c r="N41" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O41" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P41" s="8" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="A43" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C43">
-        <v>1</v>
-      </c>
-      <c r="G43">
-        <v>2</v>
-      </c>
-      <c r="N43" t="s">
-        <v>19</v>
-      </c>
-      <c r="O43" t="s">
-        <v>29</v>
-      </c>
-      <c r="P43" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q43" t="s">
+      <c r="C43" s="5">
+        <v>1</v>
+      </c>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5">
+        <v>2</v>
+      </c>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="5"/>
+      <c r="M43" s="5"/>
+      <c r="N43" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="O43" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P43" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q43" s="6" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="A44" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="N44" t="s">
-        <v>29</v>
-      </c>
-      <c r="O44" t="s">
-        <v>29</v>
-      </c>
-      <c r="P44" t="s">
-        <v>19</v>
-      </c>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8"/>
+      <c r="J44" s="8"/>
+      <c r="K44" s="8"/>
+      <c r="L44" s="8"/>
+      <c r="M44" s="8"/>
+      <c r="N44" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O44" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P44" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q44" s="9"/>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="A45" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="8">
         <v>3</v>
       </c>
-      <c r="N45" t="s">
-        <v>29</v>
-      </c>
-      <c r="O45" t="s">
-        <v>29</v>
-      </c>
-      <c r="P45" t="s">
-        <v>29</v>
-      </c>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="8"/>
+      <c r="J45" s="8"/>
+      <c r="K45" s="8"/>
+      <c r="L45" s="8"/>
+      <c r="M45" s="8"/>
+      <c r="N45" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O45" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P45" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q45" s="9"/>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="A46" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C46">
-        <v>1</v>
-      </c>
-      <c r="N46" t="s">
-        <v>29</v>
-      </c>
-      <c r="O46" t="s">
-        <v>29</v>
-      </c>
-      <c r="P46" t="s">
-        <v>19</v>
-      </c>
+      <c r="C46" s="8">
+        <v>1</v>
+      </c>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="8"/>
+      <c r="J46" s="8"/>
+      <c r="K46" s="8"/>
+      <c r="L46" s="8"/>
+      <c r="M46" s="8"/>
+      <c r="N46" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O46" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P46" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q46" s="9"/>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="A47" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="N47" t="s">
-        <v>29</v>
-      </c>
-      <c r="O47" t="s">
-        <v>29</v>
-      </c>
-      <c r="P47" t="s">
-        <v>19</v>
-      </c>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="8"/>
+      <c r="I47" s="8"/>
+      <c r="J47" s="8"/>
+      <c r="K47" s="8"/>
+      <c r="L47" s="8"/>
+      <c r="M47" s="8"/>
+      <c r="N47" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O47" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P47" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q47" s="9"/>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="A48" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C48">
-        <v>1</v>
-      </c>
-      <c r="D48">
-        <v>1</v>
-      </c>
-      <c r="G48">
-        <v>2</v>
-      </c>
-      <c r="J48">
-        <v>1</v>
-      </c>
-      <c r="K48">
-        <v>1</v>
-      </c>
-      <c r="N48" t="s">
-        <v>29</v>
-      </c>
-      <c r="O48" t="s">
-        <v>29</v>
-      </c>
-      <c r="P48" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q48" t="s">
+      <c r="C48" s="8">
+        <v>1</v>
+      </c>
+      <c r="D48" s="8">
+        <v>1</v>
+      </c>
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8">
+        <v>2</v>
+      </c>
+      <c r="H48" s="8"/>
+      <c r="I48" s="8"/>
+      <c r="J48" s="8">
+        <v>1</v>
+      </c>
+      <c r="K48" s="8">
+        <v>1</v>
+      </c>
+      <c r="L48" s="8"/>
+      <c r="M48" s="8"/>
+      <c r="N48" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O48" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P48" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q48" s="9" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="A49" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="L49">
-        <v>2</v>
-      </c>
-      <c r="N49" t="s">
-        <v>29</v>
-      </c>
-      <c r="O49" t="s">
-        <v>29</v>
-      </c>
-      <c r="P49" t="s">
-        <v>19</v>
-      </c>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="8"/>
+      <c r="J49" s="8"/>
+      <c r="K49" s="8"/>
+      <c r="L49" s="8">
+        <v>2</v>
+      </c>
+      <c r="M49" s="8"/>
+      <c r="N49" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O49" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P49" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q49" s="12"/>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="A50" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F50">
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="11">
         <v>12</v>
       </c>
-      <c r="N50" t="s">
-        <v>19</v>
-      </c>
-      <c r="O50" t="s">
-        <v>29</v>
-      </c>
-      <c r="P50" t="s">
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="11"/>
+      <c r="J50" s="11"/>
+      <c r="K50" s="11"/>
+      <c r="L50" s="11"/>
+      <c r="M50" s="11"/>
+      <c r="N50" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="O50" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="P50" s="12" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="A51" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="L51">
-        <v>2</v>
-      </c>
-      <c r="N51" t="s">
-        <v>29</v>
-      </c>
-      <c r="O51" t="s">
-        <v>29</v>
-      </c>
-      <c r="P51" t="s">
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="5"/>
+      <c r="I51" s="5"/>
+      <c r="J51" s="5"/>
+      <c r="K51" s="5"/>
+      <c r="L51" s="5">
+        <v>2</v>
+      </c>
+      <c r="M51" s="5"/>
+      <c r="N51" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O51" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P51" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="A52" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C52">
+      <c r="C52" s="11">
         <v>4</v>
       </c>
-      <c r="N52" t="s">
-        <v>29</v>
-      </c>
-      <c r="O52" t="s">
-        <v>29</v>
-      </c>
-      <c r="P52" t="s">
+      <c r="D52" s="11"/>
+      <c r="E52" s="11"/>
+      <c r="F52" s="11"/>
+      <c r="G52" s="11"/>
+      <c r="H52" s="11"/>
+      <c r="I52" s="11"/>
+      <c r="J52" s="11"/>
+      <c r="K52" s="11"/>
+      <c r="L52" s="11"/>
+      <c r="M52" s="11"/>
+      <c r="N52" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="O52" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="P52" s="12" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="A53" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C53">
+      <c r="C53" s="16">
         <v>12</v>
       </c>
-      <c r="D53">
-        <v>2</v>
-      </c>
-      <c r="H53">
-        <v>2</v>
-      </c>
-      <c r="N53" t="s">
-        <v>29</v>
-      </c>
-      <c r="O53" t="s">
-        <v>29</v>
-      </c>
-      <c r="P53" t="s">
+      <c r="D53" s="16">
+        <v>2</v>
+      </c>
+      <c r="E53" s="16"/>
+      <c r="F53" s="16"/>
+      <c r="G53" s="16"/>
+      <c r="H53" s="16">
+        <v>2</v>
+      </c>
+      <c r="I53" s="16"/>
+      <c r="J53" s="16"/>
+      <c r="K53" s="16"/>
+      <c r="L53" s="16"/>
+      <c r="M53" s="16"/>
+      <c r="N53" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="O53" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="P53" s="17" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="A54" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C54">
-        <v>2</v>
-      </c>
-      <c r="D54">
+      <c r="C54" s="5">
+        <v>2</v>
+      </c>
+      <c r="D54" s="5">
         <v>5</v>
       </c>
-      <c r="N54" t="s">
-        <v>29</v>
-      </c>
-      <c r="O54" t="s">
-        <v>29</v>
-      </c>
-      <c r="P54" t="s">
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5"/>
+      <c r="I54" s="5"/>
+      <c r="J54" s="5"/>
+      <c r="K54" s="5"/>
+      <c r="L54" s="5"/>
+      <c r="M54" s="5"/>
+      <c r="N54" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O54" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P54" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="A55" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C55">
-        <v>2</v>
-      </c>
-      <c r="D55">
-        <v>1</v>
-      </c>
-      <c r="N55" t="s">
-        <v>29</v>
-      </c>
-      <c r="O55" t="s">
-        <v>29</v>
-      </c>
-      <c r="P55" t="s">
+      <c r="C55" s="8">
+        <v>2</v>
+      </c>
+      <c r="D55" s="8">
+        <v>1</v>
+      </c>
+      <c r="E55" s="8"/>
+      <c r="F55" s="8"/>
+      <c r="G55" s="8"/>
+      <c r="H55" s="8"/>
+      <c r="I55" s="8"/>
+      <c r="J55" s="8"/>
+      <c r="K55" s="8"/>
+      <c r="L55" s="8"/>
+      <c r="M55" s="8"/>
+      <c r="N55" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O55" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P55" s="9" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="A56" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B56" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C56" s="11">
+        <v>2</v>
+      </c>
+      <c r="D56" s="11"/>
+      <c r="E56" s="11"/>
+      <c r="F56" s="11"/>
+      <c r="G56" s="11"/>
+      <c r="H56" s="11"/>
+      <c r="I56" s="11"/>
+      <c r="J56" s="11"/>
+      <c r="K56" s="11"/>
+      <c r="L56" s="11"/>
+      <c r="M56" s="11"/>
+      <c r="N56" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="O56" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="P56" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A57" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B57" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C57" s="11">
+        <v>5</v>
+      </c>
+      <c r="D57" s="11"/>
+      <c r="E57" s="11"/>
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
+      <c r="H57" s="11"/>
+      <c r="I57" s="11"/>
+      <c r="J57" s="11"/>
+      <c r="K57" s="11"/>
+      <c r="L57" s="11"/>
+      <c r="M57" s="11"/>
+      <c r="N57" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="O57" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="P57" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A58" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B58" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C56">
+      <c r="C58" s="16">
         <v>14</v>
       </c>
-      <c r="H56">
-        <v>1</v>
-      </c>
-      <c r="N56" t="s">
-        <v>29</v>
-      </c>
-      <c r="O56" t="s">
-        <v>29</v>
-      </c>
-      <c r="P56" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="D58" s="16"/>
+      <c r="E58" s="16"/>
+      <c r="F58" s="16"/>
+      <c r="G58" s="16"/>
+      <c r="H58" s="16">
+        <v>1</v>
+      </c>
+      <c r="I58" s="16"/>
+      <c r="J58" s="16"/>
+      <c r="K58" s="16"/>
+      <c r="L58" s="16"/>
+      <c r="M58" s="16"/>
+      <c r="N58" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="O58" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="P58" s="17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A59" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B59" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C57">
+      <c r="C59" s="16">
         <v>13</v>
       </c>
-      <c r="N57" t="s">
-        <v>29</v>
-      </c>
-      <c r="O57" t="s">
-        <v>29</v>
-      </c>
-      <c r="P57" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="D59" s="16"/>
+      <c r="E59" s="16"/>
+      <c r="F59" s="16"/>
+      <c r="G59" s="16"/>
+      <c r="H59" s="16"/>
+      <c r="I59" s="16"/>
+      <c r="J59" s="16"/>
+      <c r="K59" s="16"/>
+      <c r="L59" s="16"/>
+      <c r="M59" s="16"/>
+      <c r="N59" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="O59" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="P59" s="17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A60" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B60" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C58">
+      <c r="C60" s="8">
         <v>12</v>
       </c>
-      <c r="D58">
-        <v>1</v>
-      </c>
-      <c r="N58" t="s">
-        <v>29</v>
-      </c>
-      <c r="O58" t="s">
-        <v>29</v>
-      </c>
-      <c r="P58" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>94</v>
-      </c>
-      <c r="B59" t="s">
-        <v>11</v>
-      </c>
-      <c r="C59">
-        <v>5</v>
-      </c>
-      <c r="N59" t="s">
-        <v>29</v>
-      </c>
-      <c r="O59" t="s">
-        <v>29</v>
-      </c>
-      <c r="P59" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+      <c r="D60" s="8">
+        <v>1</v>
+      </c>
+      <c r="E60" s="8"/>
+      <c r="F60" s="8"/>
+      <c r="G60" s="8"/>
+      <c r="H60" s="8"/>
+      <c r="I60" s="8"/>
+      <c r="J60" s="8"/>
+      <c r="K60" s="8"/>
+      <c r="L60" s="8"/>
+      <c r="M60" s="8"/>
+      <c r="N60" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O60" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P60" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A62" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="Q60" t="s">
+      <c r="B62" s="8"/>
+      <c r="C62" s="8"/>
+      <c r="D62" s="8"/>
+      <c r="E62" s="8"/>
+      <c r="F62" s="8"/>
+      <c r="G62" s="8"/>
+      <c r="H62" s="8"/>
+      <c r="I62" s="8"/>
+      <c r="J62" s="8"/>
+      <c r="K62" s="8"/>
+      <c r="L62" s="8"/>
+      <c r="M62" s="8"/>
+      <c r="N62" s="8"/>
+      <c r="O62" s="8"/>
+      <c r="P62" s="8"/>
+      <c r="Q62" t="s">
         <v>100</v>
-      </c>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>95</v>
-      </c>
-      <c r="B61" t="s">
-        <v>11</v>
-      </c>
-      <c r="C61">
-        <v>2</v>
-      </c>
-      <c r="N61" t="s">
-        <v>29</v>
-      </c>
-      <c r="O61" t="s">
-        <v>29</v>
-      </c>
-      <c r="P61" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>16</v>
-      </c>
-      <c r="B63" t="s">
-        <v>15</v>
-      </c>
-      <c r="C63">
-        <v>6</v>
-      </c>
-      <c r="N63" t="s">
-        <v>29</v>
-      </c>
-      <c r="O63" t="s">
-        <v>29</v>
-      </c>
-      <c r="P63" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>16</v>
+      </c>
+      <c r="B65" t="s">
+        <v>15</v>
+      </c>
+      <c r="C65">
+        <v>6</v>
+      </c>
+      <c r="N65" t="s">
+        <v>29</v>
+      </c>
+      <c r="O65" t="s">
+        <v>29</v>
+      </c>
+      <c r="P65" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>74</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B67" t="s">
         <v>13</v>
       </c>
-      <c r="D65">
-        <v>2</v>
-      </c>
-      <c r="N65" t="s">
-        <v>19</v>
-      </c>
-      <c r="O65" t="s">
-        <v>29</v>
-      </c>
-      <c r="P65" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q65" t="s">
+      <c r="D67">
+        <v>2</v>
+      </c>
+      <c r="N67" t="s">
+        <v>19</v>
+      </c>
+      <c r="O67" t="s">
+        <v>29</v>
+      </c>
+      <c r="P67" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q67" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>73</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B68" t="s">
         <v>14</v>
       </c>
-      <c r="N66" t="s">
-        <v>19</v>
-      </c>
-      <c r="O66" t="s">
-        <v>29</v>
-      </c>
-      <c r="P66" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q66" t="s">
+      <c r="N68" t="s">
+        <v>19</v>
+      </c>
+      <c r="O68" t="s">
+        <v>29</v>
+      </c>
+      <c r="P68" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q68" t="s">
         <v>72</v>
       </c>
     </row>

</xml_diff>